<commit_message>
plot generation methods order changed
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>Project</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>prettyfaces</t>
+  </si>
+  <si>
+    <t>jbal</t>
+  </si>
+  <si>
+    <t>https://github.com/datazuul/jbal</t>
   </si>
 </sst>
 </file>
@@ -479,7 +485,7 @@
   <dimension ref="A4:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +680,7 @@
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>14</v>
@@ -715,7 +721,7 @@
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>21</v>
@@ -756,7 +762,7 @@
     </row>
     <row r="11" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>22</v>
@@ -797,7 +803,7 @@
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>24</v>
@@ -838,7 +844,7 @@
     </row>
     <row r="13" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>26</v>
@@ -879,7 +885,7 @@
     </row>
     <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>29</v>
@@ -920,12 +926,48 @@
     </row>
     <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="3">
+        <v>102</v>
+      </c>
+      <c r="D15" s="3">
+        <v>109</v>
+      </c>
+      <c r="E15" s="3">
+        <v>113</v>
+      </c>
+      <c r="F15" s="3">
+        <v>370</v>
+      </c>
+      <c r="G15" s="3">
+        <v>28</v>
+      </c>
+      <c r="H15" s="3">
+        <v>250</v>
+      </c>
+      <c r="I15" s="3">
+        <v>4678</v>
+      </c>
+      <c r="J15" s="3">
+        <v>4700</v>
+      </c>
+      <c r="K15" s="3">
+        <v>88</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -935,6 +977,7 @@
     <hyperlink ref="M12" r:id="rId3"/>
     <hyperlink ref="M13" r:id="rId4"/>
     <hyperlink ref="M14" r:id="rId5"/>
+    <hyperlink ref="M15" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
avoid overwriting same name xml files
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
   <si>
     <t>Project</t>
   </si>
@@ -142,13 +142,43 @@
   </si>
   <si>
     <t>https://github.com/xebia-france/selma</t>
+  </si>
+  <si>
+    <t>https://github.com/hcarver/bluecove</t>
+  </si>
+  <si>
+    <t>bluecove</t>
+  </si>
+  <si>
+    <t>gp-net-radius</t>
+  </si>
+  <si>
+    <t>https://github.com/GegeFR/gp-net-radius</t>
+  </si>
+  <si>
+    <t>aima-java</t>
+  </si>
+  <si>
+    <t>https://github.com/aimacode/aima-java</t>
+  </si>
+  <si>
+    <t>https://github.com/powermock/powermock</t>
+  </si>
+  <si>
+    <t>powermock</t>
+  </si>
+  <si>
+    <t>https://github.com/restfb/restfb</t>
+  </si>
+  <si>
+    <t>restfb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +205,13 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -217,14 +254,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -527,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:M21"/>
+  <dimension ref="A4:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,141 +1089,255 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>9</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>240</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>158</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>280</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>571</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <v>250</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <v>1582</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="5">
         <v>4182</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="5">
         <v>4600</v>
       </c>
-      <c r="K17" s="6">
+      <c r="K17" s="5">
         <v>133</v>
       </c>
-      <c r="L17" s="6" t="s">
+      <c r="L17" s="5" t="s">
         <v>16</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>10</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>309</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>118</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>743</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <v>988</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <v>1562</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <v>3051</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="5">
         <v>21491</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="5">
         <v>22701</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="5">
         <v>347</v>
       </c>
-      <c r="L18" s="6" t="s">
+      <c r="L18" s="5" t="s">
         <v>16</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>11</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>21</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>22</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>81</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <v>32</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <v>64</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="5">
         <v>180</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="5">
         <v>38</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="5">
         <v>241</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="5">
         <v>13</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>12</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>368</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="M20" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>13</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7">
+        <v>1679</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>14</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7">
+        <v>28</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>15</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7">
+        <v>1181</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>16</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1512</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>17</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1545</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M10" r:id="rId1"/>
@@ -1199,9 +1351,14 @@
     <hyperlink ref="M18" r:id="rId9"/>
     <hyperlink ref="M19" r:id="rId10"/>
     <hyperlink ref="M20" r:id="rId11"/>
+    <hyperlink ref="M21" r:id="rId12"/>
+    <hyperlink ref="M22" r:id="rId13"/>
+    <hyperlink ref="M23" r:id="rId14"/>
+    <hyperlink ref="M24" r:id="rId15"/>
+    <hyperlink ref="M25" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>